<commit_message>
Update scenario projections and shiny app
</commit_message>
<xml_diff>
--- a/RSV-Scenarios-Shiny-App/effectiveness_parameters.xlsx
+++ b/RSV-Scenarios-Shiny-App/effectiveness_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih-my.sharepoint.com/personal/hansencl_nih_gov1/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih-my.sharepoint.com/personal/hansencl_nih_gov1/Documents/Documents/RProjects on github/RSV Interventions/RSV-Scenarios-Shiny-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26A40CE5-ABE2-4733-9B17-C01BD71657F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{26A40CE5-ABE2-4733-9B17-C01BD71657F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06CD698A-9D67-4443-92FA-7686D3E88361}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00101E46-7C5F-48A5-A5E1-93EC2D0A6BA1}"/>
+    <workbookView xWindow="780" yWindow="1995" windowWidth="21600" windowHeight="10890" xr2:uid="{00101E46-7C5F-48A5-A5E1-93EC2D0A6BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Scenario</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Senior Vaccination</t>
   </si>
   <si>
-    <t>Optimistic Scenario</t>
-  </si>
-  <si>
-    <t>Pessimistic Scenario</t>
-  </si>
-  <si>
     <t>Duration of Protection</t>
   </si>
   <si>
@@ -68,16 +62,13 @@
     <t>80%</t>
   </si>
   <si>
-    <t>70%</t>
-  </si>
-  <si>
-    <t>90%</t>
-  </si>
-  <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>50%</t>
+    <t>150 days</t>
+  </si>
+  <si>
+    <t>55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effectiveness </t>
   </si>
 </sst>
 </file>
@@ -450,20 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66A1750-DFCE-45AD-851C-F0542C438EF3}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,46 +468,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>